<commit_message>
Tests de caja negra implementados, excel modificado
</commit_message>
<xml_diff>
--- a/practica4/Informe.xlsx
+++ b/practica4/Informe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicancloud-my.sharepoint.com/personal/jlf799_alumnos_unican_es/Documents/UNICAN/SoftwareII/Practicas/GIT/IS2_2021/practica4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\IS2_2021\practica4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="299" documentId="11_AD4D2F04E46CFB4ACB3E20499DD7E574683EDF25" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FF72672B-FB00-42CC-9B9D-50D199003367}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5D5779-4816-4A4A-9FC3-DE53AC85B81A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CajaNegra" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="41">
   <si>
     <t>Casos de prueba valido</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Potencia</t>
   </si>
   <si>
-    <t>Tipo Seguro</t>
-  </si>
-  <si>
     <t>Siniestro</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>(110,inf)</t>
   </si>
   <si>
-    <t>Seguro</t>
-  </si>
-  <si>
     <t>Valor</t>
   </si>
   <si>
@@ -160,10 +154,10 @@
     <t>cliente</t>
   </si>
   <si>
-    <t>Excepcion</t>
-  </si>
-  <si>
     <t>Se crea el cliente</t>
+  </si>
+  <si>
+    <t>Cobertura</t>
   </si>
 </sst>
 </file>
@@ -218,13 +212,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -506,22 +501,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -529,12 +525,12 @@
         <v>400</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -543,12 +539,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -560,19 +556,19 @@
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -586,25 +582,25 @@
         <v>1</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M4">
         <f>(D15+D10)</f>
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>1.2</v>
@@ -613,62 +609,62 @@
         <v>50</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M5">
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="I6">
         <v>89</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M6">
         <f>(D$9*D$3+D$17)*D$22</f>
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4"/>
       <c r="I7">
         <v>90</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M7">
         <f>(D$9*D$4+D$17)*D$22</f>
         <v>465</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
@@ -680,25 +676,25 @@
         <v>110</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M8">
         <f>1000*1.05+50</f>
         <v>1100</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -710,28 +706,28 @@
         <v>110</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M9">
         <f>(D$9*D$4+D$17)*D$22</f>
         <v>465</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
       </c>
       <c r="D10">
         <v>600</v>
@@ -740,25 +736,25 @@
         <v>111</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M10">
         <f>(D$9*D$5+D$17)*D$22</f>
         <v>510</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>1000</v>
@@ -767,33 +763,33 @@
         <v>120</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M11">
         <f>1200+50</f>
         <v>1250</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>0</v>
@@ -803,12 +799,12 @@
       </c>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -818,44 +814,45 @@
       </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="D16">
         <v>50</v>
       </c>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>200</v>
       </c>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="1"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>0</v>
@@ -865,12 +862,12 @@
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -881,12 +878,12 @@
       <c r="J21" s="4"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -896,25 +893,25 @@
       </c>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
@@ -926,21 +923,21 @@
         <v>7</v>
       </c>
       <c r="J30" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K30" t="s">
+        <v>32</v>
+      </c>
+      <c r="L30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="L30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
@@ -949,50 +946,50 @@
         <v>100</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>6</v>
       </c>
       <c r="L31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I32">
         <v>-1</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K32" t="s">
+        <v>38</v>
+      </c>
+      <c r="L32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>40</v>
-      </c>
-      <c r="L32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>6</v>
       </c>
       <c r="L33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>0</v>
@@ -1007,18 +1004,18 @@
         <v>6</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
@@ -1027,50 +1024,50 @@
         <v>100</v>
       </c>
       <c r="J35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="C36" t="s">
         <v>17</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" t="s">
-        <v>18</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="J38" s="5"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>0</v>
@@ -1079,23 +1076,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="M8" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1105,7 +1105,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>